<commit_message>
add subset function "calculate_transaction_metrics"
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F62463-D3C6-4DD4-BEAC-A59316DCC413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE6F7E0-2361-4D5E-93C9-CAE812EFC74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="2175" windowWidth="22485" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>BLKRK</t>
+  </si>
+  <si>
+    <t>broker</t>
+  </si>
+  <si>
+    <t>company_a</t>
+  </si>
+  <si>
+    <t>company_b</t>
+  </si>
+  <si>
+    <t>NFLX</t>
   </si>
 </sst>
 </file>
@@ -493,444 +505,553 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2">
         <v>44074</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>6.1519532451553367</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>325.10000000000002</v>
       </c>
-      <c r="F2">
-        <f>D2*E2</f>
+      <c r="G2">
+        <f>E2*F2</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
         <v>44222</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>102.19724067450178</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>19.57</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F12" si="0">D3*E3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="0">E3*F3</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
         <v>44253</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>21.072595090085343</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>94.91</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>1999.9999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
         <v>44354</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>62</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>32.159999999999997</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>1993.9199999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
         <v>44378</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
-        <v>21</v>
-      </c>
       <c r="E6">
+        <v>21</v>
+      </c>
+      <c r="F6">
         <v>93.31</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>1959.51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
         <v>44378</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>24.965672200724004</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>80.11</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
         <v>44405</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>61.425061425061422</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>32.56</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
         <v>44413</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
       <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>88.80994671403198</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>22.52</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>2000.0000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
         <v>44473</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
       <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>82.850041425020706</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>24.14</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>1999.9999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
         <v>44480</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
       <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>9.6641700893935738</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>206.95</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
         <v>44487</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
       <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>18.181818181818183</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>110</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>2000.0000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
         <v>44659</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>-15</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>101</v>
       </c>
-      <c r="F13">
-        <f t="shared" ref="F13" si="1">D13*E13</f>
+      <c r="G13">
+        <f t="shared" ref="G13" si="1">E13*F13</f>
         <v>-1515</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
         <v>44665</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
       <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>95</v>
       </c>
-      <c r="F14">
-        <f t="shared" ref="F14" si="2">D14*E14</f>
+      <c r="G14">
+        <f t="shared" ref="G14" si="2">E14*F14</f>
         <v>950</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
         <v>44673</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>-5</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>101</v>
       </c>
-      <c r="F15">
-        <f t="shared" ref="F15:F17" si="3">D15*E15</f>
+      <c r="G15">
+        <f t="shared" ref="G15:G17" si="3">E15*F15</f>
         <v>-505</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
         <v>44680</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
       <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>5</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>110</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <f t="shared" si="3"/>
         <v>550</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
         <v>44687</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-62</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>50</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f t="shared" si="3"/>
         <v>-3100</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
         <v>44691</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>5</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>10</v>
       </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F19" si="4">D18*E18</f>
+      <c r="G18">
+        <f t="shared" ref="G18:G19" si="4">E18*F18</f>
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2">
         <v>44693</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
       <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>5</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>12</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
         <v>44697</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
       <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>5</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>14</v>
       </c>
-      <c r="F20">
-        <f t="shared" ref="F20" si="5">D20*E20</f>
+      <c r="G20">
+        <f t="shared" ref="G20" si="5">E20*F20</f>
         <v>70</v>
       </c>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>186.35</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G22" si="6">E21*F21</f>
+        <v>931.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>44722</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>182.94</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>914.7</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F9">
+    <sortCondition ref="B1:B9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change class name to `Portfolio`
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE6F7E0-2361-4D5E-93C9-CAE812EFC74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6FC4B8-8790-44C4-9E30-0D78D26DDB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="2175" windowWidth="22485" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>NFLX</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
@@ -161,12 +164,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -550,23 +556,15 @@
         <v>21</v>
       </c>
       <c r="B2" s="2">
-        <v>44074</v>
+        <v>44073</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>6.1519532451553367</v>
-      </c>
-      <c r="F2">
-        <v>325.10000000000002</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2">
-        <f>E2*F2</f>
-        <v>2000</v>
+        <v>-21953.43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -574,22 +572,22 @@
         <v>21</v>
       </c>
       <c r="B3" s="2">
-        <v>44222</v>
+        <v>44074</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>102.19724067450178</v>
+        <v>6.1519532451553367</v>
       </c>
       <c r="F3">
-        <v>19.57</v>
+        <v>325.10000000000002</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">E3*F3</f>
+        <f>E3*F3</f>
         <v>2000</v>
       </c>
     </row>
@@ -598,115 +596,115 @@
         <v>21</v>
       </c>
       <c r="B4" s="2">
+        <v>44222</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>102.19724067450178</v>
+      </c>
+      <c r="F4">
+        <v>19.57</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G13" si="0">E4*F4</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
         <v>44253</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>21.072595090085343</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>94.91</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>1999.9999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
         <v>44354</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>62</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>32.159999999999997</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>1993.9199999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
         <v>44378</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E6">
-        <v>21</v>
-      </c>
-      <c r="F6">
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="F7">
         <v>93.31</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>1959.51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44378</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>24.965672200724004</v>
-      </c>
-      <c r="F7">
-        <v>80.11</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2">
-        <v>44405</v>
+        <v>44378</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>61.425061425061422</v>
+        <v>24.965672200724004</v>
       </c>
       <c r="F8">
-        <v>32.56</v>
+        <v>80.11</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -718,23 +716,23 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>44413</v>
+        <v>44405</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>88.80994671403198</v>
+        <v>61.425061425061422</v>
       </c>
       <c r="F9">
-        <v>22.52</v>
+        <v>32.56</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>2000.0000000000002</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -742,23 +740,23 @@
         <v>21</v>
       </c>
       <c r="B10" s="2">
-        <v>44473</v>
+        <v>44413</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>82.850041425020706</v>
+        <v>88.80994671403198</v>
       </c>
       <c r="F10">
-        <v>24.14</v>
+        <v>22.52</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>1999.9999999999998</v>
+        <v>2000.0000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -766,23 +764,23 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>44480</v>
+        <v>44473</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11">
-        <v>9.6641700893935738</v>
+        <v>82.850041425020706</v>
       </c>
       <c r="F11">
-        <v>206.95</v>
+        <v>24.14</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1999.9999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -790,23 +788,23 @@
         <v>21</v>
       </c>
       <c r="B12" s="2">
-        <v>44487</v>
+        <v>44480</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E12">
-        <v>18.181818181818183</v>
+        <v>9.6641700893935738</v>
       </c>
       <c r="F12">
-        <v>110</v>
+        <v>206.95</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>2000.0000000000002</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -814,23 +812,23 @@
         <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>44659</v>
+        <v>44487</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E13">
-        <v>-15</v>
+        <v>18.181818181818183</v>
       </c>
       <c r="F13">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13" si="1">E13*F13</f>
-        <v>-1515</v>
+        <f t="shared" si="0"/>
+        <v>2000.0000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -838,23 +836,23 @@
         <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>44665</v>
+        <v>44659</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>-15</v>
       </c>
       <c r="F14">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14" si="2">E14*F14</f>
-        <v>950</v>
+        <f t="shared" ref="G14" si="1">E14*F14</f>
+        <v>-1515</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -862,23 +860,23 @@
         <v>21</v>
       </c>
       <c r="B15" s="2">
-        <v>44673</v>
+        <v>44665</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G17" si="3">E15*F15</f>
-        <v>-505</v>
+        <f t="shared" ref="G15" si="2">E15*F15</f>
+        <v>950</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -886,79 +884,79 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>44680</v>
+        <v>44673</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16">
+        <v>-5</v>
+      </c>
+      <c r="F16">
+        <v>101</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G18" si="3">E16*F16</f>
+        <v>-505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44680</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>110</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <f t="shared" si="3"/>
         <v>550</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
         <v>44687</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>-62</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>50</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <f t="shared" si="3"/>
         <v>-3100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="2">
-        <v>44691</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ref="G18:G19" si="4">E18*F18</f>
-        <v>50</v>
-      </c>
-    </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>44693</v>
+        <v>44691</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -970,59 +968,59 @@
         <v>5</v>
       </c>
       <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G20" si="4">E19*F19</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44693</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
         <v>12</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2">
-        <v>44697</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20">
-        <v>5</v>
-      </c>
-      <c r="F20">
-        <v>14</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ref="G20" si="5">E20*F20</f>
-        <v>70</v>
-      </c>
-    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>44701</v>
+        <v>44697</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21">
-        <v>186.35</v>
+        <v>14</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G22" si="6">E21*F21</f>
-        <v>931.75</v>
+        <f t="shared" ref="G21" si="5">E21*F21</f>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1030,10 +1028,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>44722</v>
+        <v>44701</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
@@ -1042,16 +1040,40 @@
         <v>5</v>
       </c>
       <c r="F22">
+        <v>186.35</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G23" si="6">E22*F22</f>
+        <v>931.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44722</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
         <v>182.94</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <f t="shared" si="6"/>
         <v>914.7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F9">
-    <sortCondition ref="B1:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F10">
+    <sortCondition ref="B1:B10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add cash and update tests
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6FC4B8-8790-44C4-9E30-0D78D26DDB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E722E-156E-4423-B379-80A4D241148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -164,15 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -526,9 +526,11 @@
     <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -551,7 +553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -561,13 +563,22 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>21953.43</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="G2">
-        <v>-21953.43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C2="Cash",1,-1)*E2*F2</f>
+        <v>21953.43</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -587,11 +598,12 @@
         <v>325.10000000000002</v>
       </c>
       <c r="G3">
-        <f>E3*F3</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C3="Cash",1,-1)*E3*F3</f>
+        <v>-2000</v>
+      </c>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -611,11 +623,12 @@
         <v>19.57</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G13" si="0">E4*F4</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C4="Cash",1,-1)*E4*F4</f>
+        <v>-2000</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -635,256 +648,266 @@
         <v>94.91</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>1999.9999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C5="Cash",1,-1)*E5*F5</f>
+        <v>-1999.9999999999998</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2">
+        <v>44328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <f>IF(C7="Cash",1,-1)*E7*F7</f>
+        <v>-50</v>
+      </c>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
         <v>44354</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>62</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>32.159999999999997</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1993.9199999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="G8">
+        <f>IF(C8="Cash",1,-1)*E8*F8</f>
+        <v>-1993.9199999999998</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
         <v>44378</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E7">
-        <v>21</v>
-      </c>
-      <c r="F7">
+      <c r="E9">
+        <v>21</v>
+      </c>
+      <c r="F9">
         <v>93.31</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1959.51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="G9">
+        <f>IF(C9="Cash",1,-1)*E9*F9</f>
+        <v>-1959.51</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
         <v>44378</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>24.965672200724004</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>80.11</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="G10">
+        <f>IF(C10="Cash",1,-1)*E10*F10</f>
+        <v>-2000</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
         <v>44405</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>61.425061425061422</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>32.56</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="G11">
+        <f>IF(C11="Cash",1,-1)*E11*F11</f>
+        <v>-2000</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
         <v>44413</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>88.80994671403198</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <v>22.52</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>2000.0000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="G12">
+        <f>IF(C12="Cash",1,-1)*E12*F12</f>
+        <v>-2000.0000000000002</v>
+      </c>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
         <v>44473</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E11">
+      <c r="E13">
         <v>82.850041425020706</v>
       </c>
-      <c r="F11">
+      <c r="F13">
         <v>24.14</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>1999.9999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="G13">
+        <f>IF(C13="Cash",1,-1)*E13*F13</f>
+        <v>-1999.9999999999998</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
         <v>44480</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>9.6641700893935738</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <v>206.95</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="G14">
+        <f>IF(C14="Cash",1,-1)*E14*F14</f>
+        <v>-2000</v>
+      </c>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
         <v>44487</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>18.181818181818183</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>110</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>2000.0000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="G15">
+        <f>IF(C15="Cash",1,-1)*E15*F15</f>
+        <v>-2000.0000000000002</v>
+      </c>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
         <v>44659</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>-15</v>
-      </c>
-      <c r="F14">
-        <v>101</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ref="G14" si="1">E14*F14</f>
-        <v>-1515</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2">
-        <v>44665</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>95</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ref="G15" si="2">E15*F15</f>
-        <v>950</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2">
-        <v>44673</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -893,22 +916,23 @@
         <v>6</v>
       </c>
       <c r="E16">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="F16">
         <v>101</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G18" si="3">E16*F16</f>
-        <v>-505</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C16="Cash",1,-1)*E16*F16</f>
+        <v>1515</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>44680</v>
+        <v>44665</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -917,163 +941,243 @@
         <v>6</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
-        <v>550</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C17="Cash",1,-1)*E17*F17</f>
+        <v>-950</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>44687</v>
+        <v>44673</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>-62</v>
+        <v>-5</v>
       </c>
       <c r="F18">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>-3100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+        <f>IF(C18="Cash",1,-1)*E18*F18</f>
+        <v>505</v>
+      </c>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>44691</v>
+        <v>44680</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G20" si="4">E19*F19</f>
+        <f>IF(C19="Cash",1,-1)*E19*F19</f>
+        <v>-550</v>
+      </c>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44687</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <v>-62</v>
+      </c>
+      <c r="F20">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2">
+      <c r="G20">
+        <f>IF(C20="Cash",1,-1)*E20*F20</f>
+        <v>3100</v>
+      </c>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
         <v>44693</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>70</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>70</v>
+      </c>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>44693</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
-      </c>
-      <c r="E20">
-        <v>5</v>
-      </c>
-      <c r="F20">
-        <v>12</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>44697</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21">
-        <v>14</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ref="G21" si="5">E21*F21</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>44701</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <f>IF(C22="Cash",1,-1)*E22*F22</f>
+        <v>-70</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <v>-1000</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f>IF(C23="Cash",1,-1)*E23*F23</f>
+        <v>-1000</v>
+      </c>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>1000</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f>IF(C24="Cash",1,-1)*E24*F24</f>
+        <v>1000</v>
+      </c>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
         <v>186.35</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:G23" si="6">E22*F22</f>
-        <v>931.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
+      <c r="G25">
+        <f>IF(C25="Cash",1,-1)*E25*F25</f>
+        <v>-931.75</v>
+      </c>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B26" s="2">
         <v>44722</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>18</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="E23">
-        <v>5</v>
-      </c>
-      <c r="F23">
+      <c r="E26">
+        <v>-5</v>
+      </c>
+      <c r="F26">
         <v>182.94</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="6"/>
+      <c r="G26">
+        <f>IF(C26="Cash",1,-1)*E26*F26</f>
         <v>914.7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F10">
-    <sortCondition ref="B1:B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F11">
+    <sortCondition ref="B1:B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding insider transactions and benchmark
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E722E-156E-4423-B379-80A4D241148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60693B1-B9DB-4D75-AA45-4C861DA24721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="383" windowWidth="22485" windowHeight="11864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -558,7 +558,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2">
-        <v>44073</v>
+        <v>44074</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -697,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <f>IF(C7="Cash",1,-1)*E7*F7</f>
+        <f t="shared" ref="G7:G20" si="0">IF(C7="Cash",1,-1)*E7*F7</f>
         <v>-50</v>
       </c>
       <c r="O7" s="2"/>
@@ -722,7 +722,7 @@
         <v>32.159999999999997</v>
       </c>
       <c r="G8">
-        <f>IF(C8="Cash",1,-1)*E8*F8</f>
+        <f t="shared" si="0"/>
         <v>-1993.9199999999998</v>
       </c>
       <c r="O8" s="2"/>
@@ -747,7 +747,7 @@
         <v>93.31</v>
       </c>
       <c r="G9">
-        <f>IF(C9="Cash",1,-1)*E9*F9</f>
+        <f t="shared" si="0"/>
         <v>-1959.51</v>
       </c>
       <c r="O9" s="2"/>
@@ -772,7 +772,7 @@
         <v>80.11</v>
       </c>
       <c r="G10">
-        <f>IF(C10="Cash",1,-1)*E10*F10</f>
+        <f t="shared" si="0"/>
         <v>-2000</v>
       </c>
       <c r="O10" s="2"/>
@@ -797,7 +797,7 @@
         <v>32.56</v>
       </c>
       <c r="G11">
-        <f>IF(C11="Cash",1,-1)*E11*F11</f>
+        <f t="shared" si="0"/>
         <v>-2000</v>
       </c>
       <c r="O11" s="2"/>
@@ -822,7 +822,7 @@
         <v>22.52</v>
       </c>
       <c r="G12">
-        <f>IF(C12="Cash",1,-1)*E12*F12</f>
+        <f t="shared" si="0"/>
         <v>-2000.0000000000002</v>
       </c>
       <c r="O12" s="2"/>
@@ -847,7 +847,7 @@
         <v>24.14</v>
       </c>
       <c r="G13">
-        <f>IF(C13="Cash",1,-1)*E13*F13</f>
+        <f t="shared" si="0"/>
         <v>-1999.9999999999998</v>
       </c>
       <c r="O13" s="2"/>
@@ -872,7 +872,7 @@
         <v>206.95</v>
       </c>
       <c r="G14">
-        <f>IF(C14="Cash",1,-1)*E14*F14</f>
+        <f t="shared" si="0"/>
         <v>-2000</v>
       </c>
       <c r="O14" s="2"/>
@@ -897,7 +897,7 @@
         <v>110</v>
       </c>
       <c r="G15">
-        <f>IF(C15="Cash",1,-1)*E15*F15</f>
+        <f t="shared" si="0"/>
         <v>-2000.0000000000002</v>
       </c>
       <c r="O15" s="2"/>
@@ -922,7 +922,7 @@
         <v>101</v>
       </c>
       <c r="G16">
-        <f>IF(C16="Cash",1,-1)*E16*F16</f>
+        <f t="shared" si="0"/>
         <v>1515</v>
       </c>
       <c r="O16" s="2"/>
@@ -947,7 +947,7 @@
         <v>95</v>
       </c>
       <c r="G17">
-        <f>IF(C17="Cash",1,-1)*E17*F17</f>
+        <f t="shared" si="0"/>
         <v>-950</v>
       </c>
       <c r="O17" s="2"/>
@@ -972,7 +972,7 @@
         <v>101</v>
       </c>
       <c r="G18">
-        <f>IF(C18="Cash",1,-1)*E18*F18</f>
+        <f t="shared" si="0"/>
         <v>505</v>
       </c>
       <c r="O18" s="2"/>
@@ -997,7 +997,7 @@
         <v>110</v>
       </c>
       <c r="G19">
-        <f>IF(C19="Cash",1,-1)*E19*F19</f>
+        <f t="shared" si="0"/>
         <v>-550</v>
       </c>
       <c r="O19" s="2"/>
@@ -1022,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="G20">
-        <f>IF(C20="Cash",1,-1)*E20*F20</f>
+        <f t="shared" si="0"/>
         <v>3100</v>
       </c>
       <c r="O20" s="2"/>

</xml_diff>

<commit_message>
handle zero for heatmap and add tests
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60693B1-B9DB-4D75-AA45-4C861DA24721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F08D7DC-B186-4746-AB39-40E89252503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="383" windowWidth="22485" windowHeight="11864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>Cash</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>CCIV</t>
+  </si>
+  <si>
+    <t>delisted</t>
+  </si>
+  <si>
+    <t>stock split</t>
+  </si>
+  <si>
+    <t>fund</t>
+  </si>
+  <si>
+    <t>BOOK</t>
   </si>
 </sst>
 </file>
@@ -511,17 +529,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
@@ -552,6 +570,9 @@
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
@@ -697,8 +718,11 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G20" si="0">IF(C7="Cash",1,-1)*E7*F7</f>
+        <f>IF(C7="Cash",1,-1)*E7*F7</f>
         <v>-50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
       </c>
       <c r="O7" s="2"/>
     </row>
@@ -722,7 +746,7 @@
         <v>32.159999999999997</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>IF(C8="Cash",1,-1)*E8*F8</f>
         <v>-1993.9199999999998</v>
       </c>
       <c r="O8" s="2"/>
@@ -747,7 +771,7 @@
         <v>93.31</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f>IF(C9="Cash",1,-1)*E9*F9</f>
         <v>-1959.51</v>
       </c>
       <c r="O9" s="2"/>
@@ -772,7 +796,7 @@
         <v>80.11</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>IF(C10="Cash",1,-1)*E10*F10</f>
         <v>-2000</v>
       </c>
       <c r="O10" s="2"/>
@@ -797,7 +821,7 @@
         <v>32.56</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f>IF(C11="Cash",1,-1)*E11*F11</f>
         <v>-2000</v>
       </c>
       <c r="O11" s="2"/>
@@ -822,7 +846,7 @@
         <v>22.52</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f>IF(C12="Cash",1,-1)*E12*F12</f>
         <v>-2000.0000000000002</v>
       </c>
       <c r="O12" s="2"/>
@@ -847,7 +871,7 @@
         <v>24.14</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f>IF(C13="Cash",1,-1)*E13*F13</f>
         <v>-1999.9999999999998</v>
       </c>
       <c r="O13" s="2"/>
@@ -872,7 +896,7 @@
         <v>206.95</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>IF(C14="Cash",1,-1)*E14*F14</f>
         <v>-2000</v>
       </c>
       <c r="O14" s="2"/>
@@ -897,7 +921,7 @@
         <v>110</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f>IF(C15="Cash",1,-1)*E15*F15</f>
         <v>-2000.0000000000002</v>
       </c>
       <c r="O15" s="2"/>
@@ -907,23 +931,26 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>44659</v>
+        <v>44488</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E16">
-        <v>-15</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>1515</v>
+        <f>IF(C16="Cash",1,-1)*E16*F16</f>
+        <v>-100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
       </c>
       <c r="O16" s="2"/>
     </row>
@@ -932,23 +959,26 @@
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>44665</v>
+        <v>44489</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F17">
-        <v>95</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>-950</v>
+        <f>IF(C17="Cash",1,-1)*E17*F17</f>
+        <v>102</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
       </c>
       <c r="O17" s="2"/>
     </row>
@@ -957,7 +987,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>44673</v>
+        <v>44659</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -966,14 +996,14 @@
         <v>6</v>
       </c>
       <c r="E18">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="F18">
         <v>101</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>505</v>
+        <f>IF(C18="Cash",1,-1)*E18*F18</f>
+        <v>1515</v>
       </c>
       <c r="O18" s="2"/>
     </row>
@@ -982,7 +1012,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>44680</v>
+        <v>44665</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -991,14 +1021,14 @@
         <v>6</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
-        <v>-550</v>
+        <f>IF(C19="Cash",1,-1)*E19*F19</f>
+        <v>-950</v>
       </c>
       <c r="O19" s="2"/>
     </row>
@@ -1007,23 +1037,23 @@
         <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>44687</v>
+        <v>44673</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>-62</v>
+        <v>-5</v>
       </c>
       <c r="F20">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>3100</v>
+        <f>IF(C20="Cash",1,-1)*E20*F20</f>
+        <v>505</v>
       </c>
       <c r="O20" s="2"/>
     </row>
@@ -1032,22 +1062,23 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>44693</v>
+        <v>44680</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="G21">
-        <v>70</v>
+        <f>IF(C21="Cash",1,-1)*E21*F21</f>
+        <v>-550</v>
       </c>
       <c r="O21" s="2"/>
     </row>
@@ -1056,23 +1087,23 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>44693</v>
+        <v>44687</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>-62</v>
       </c>
       <c r="F22">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G22">
         <f>IF(C22="Cash",1,-1)*E22*F22</f>
-        <v>-70</v>
+        <v>3100</v>
       </c>
       <c r="O22" s="2"/>
     </row>
@@ -1081,7 +1112,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>44701</v>
+        <v>44693</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
@@ -1090,48 +1121,50 @@
         <v>24</v>
       </c>
       <c r="E23">
-        <v>-1000</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <f>IF(C23="Cash",1,-1)*E23*F23</f>
-        <v>-1000</v>
+        <v>70</v>
       </c>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
-        <v>44701</v>
+        <v>44693</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E24">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G24">
         <f>IF(C24="Cash",1,-1)*E24*F24</f>
-        <v>1000</v>
+        <v>-70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>29</v>
       </c>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2">
-        <v>44701</v>
+        <v>44700</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1153,29 +1186,156 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
-        <v>44722</v>
+        <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26">
-        <v>-5</v>
+        <v>-1000</v>
       </c>
       <c r="F26">
-        <v>182.94</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f>IF(C26="Cash",1,-1)*E26*F26</f>
-        <v>914.7</v>
-      </c>
-    </row>
+        <v>-1000</v>
+      </c>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27">
+        <v>1000</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f>IF(C27="Cash",1,-1)*E27*F27</f>
+        <v>1000</v>
+      </c>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>186.35</v>
+      </c>
+      <c r="G28">
+        <f>IF(C28="Cash",1,-1)*E28*F28</f>
+        <v>-931.75</v>
+      </c>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44702</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44702</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44722</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>182.94</v>
+      </c>
+      <c r="G31">
+        <f>IF(C31="Cash",1,-1)*E31*F31</f>
+        <v>-914.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
+  <autoFilter ref="A1:H31" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
+      <sortCondition ref="B1:B31"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F11">
     <sortCondition ref="B1:B11"/>
   </sortState>

</xml_diff>

<commit_message>
support selling in benchmark
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F67F39-5AD1-428A-83C7-202D88333F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB8605-060D-4E7A-85E4-EFD996B65D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="2205" windowWidth="22485" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>SELL</t>
+  </si>
+  <si>
+    <t>withdrawal</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1145,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="G24">
-        <f>IF(C24="Cash",1,-1)*E24*F24</f>
+        <f t="shared" ref="G24:G28" si="1">IF(C24="Cash",1,-1)*E24*F24</f>
         <v>-70</v>
       </c>
       <c r="H24" t="s">
@@ -1173,7 +1176,7 @@
         <v>186.35</v>
       </c>
       <c r="G25">
-        <f>IF(C25="Cash",1,-1)*E25*F25</f>
+        <f t="shared" si="1"/>
         <v>-931.75</v>
       </c>
       <c r="O25" s="2"/>
@@ -1198,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <f>IF(C26="Cash",1,-1)*E26*F26</f>
+        <f t="shared" si="1"/>
         <v>-1000</v>
       </c>
       <c r="O26" s="2"/>
@@ -1223,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <f>IF(C27="Cash",1,-1)*E27*F27</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="O27" s="2"/>
@@ -1248,33 +1251,36 @@
         <v>186.35</v>
       </c>
       <c r="G28">
-        <f>IF(C28="Cash",1,-1)*E28*F28</f>
+        <f t="shared" si="1"/>
         <v>-931.75</v>
       </c>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2">
-        <v>44722</v>
+        <v>44704</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E29">
-        <v>-5</v>
+        <v>-1000</v>
       </c>
       <c r="F29">
-        <v>182.94</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <f>IF(C29="Cash",1,-1)*E29*F29</f>
-        <v>914.7</v>
+        <f t="shared" ref="G29" si="2">IF(C29="Cash",1,-1)*E29*F29</f>
+        <v>-1000</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stock calendar check and benchmark test
</commit_message>
<xml_diff>
--- a/tests/files/test_transactions.xlsx
+++ b/tests/files/test_transactions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB8605-060D-4E7A-85E4-EFD996B65D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6303BEAD-4383-4309-A483-20F59EF5E4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="2205" windowWidth="22485" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1186,7 +1186,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="2">
-        <v>44701</v>
+        <v>44700</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
@@ -1284,7 +1284,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H28" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F11">
     <sortCondition ref="B1:B11"/>
   </sortState>

</xml_diff>